<commit_message>
ajout semaines de vacance
</commit_message>
<xml_diff>
--- a/EE04.xlsx
+++ b/EE04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olimo\remise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1696BA-6063-4C58-9F79-17101E09447D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EC7682-01A6-4602-99E1-7571CD1AAC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1699,6 +1699,118 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -1707,26 +1819,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1751,85 +1843,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1843,8 +1859,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1855,49 +1883,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2274,41 +2274,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="19.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="107"/>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="107"/>
-      <c r="AE2" s="107"/>
-      <c r="AF2" s="107"/>
-      <c r="AG2" s="107"/>
-      <c r="AH2" s="107"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="101"/>
+      <c r="AA2" s="101"/>
+      <c r="AB2" s="101"/>
+      <c r="AC2" s="101"/>
+      <c r="AD2" s="101"/>
+      <c r="AE2" s="101"/>
+      <c r="AF2" s="101"/>
+      <c r="AG2" s="101"/>
+      <c r="AH2" s="101"/>
     </row>
     <row r="3" spans="2:34" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -2319,122 +2319,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="L5" s="109" t="s">
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="L5" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="109"/>
-      <c r="N5" s="109"/>
-      <c r="O5" s="109"/>
-      <c r="P5" s="109"/>
-      <c r="R5" s="110" t="s">
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="R5" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="110"/>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
-      <c r="Y5" s="110"/>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="110"/>
-      <c r="AB5" s="110"/>
-      <c r="AC5" s="110"/>
-      <c r="AD5" s="110"/>
-      <c r="AE5" s="110"/>
-      <c r="AF5" s="110"/>
-      <c r="AG5" s="110"/>
-      <c r="AH5" s="110"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="107"/>
+      <c r="W5" s="107"/>
+      <c r="X5" s="107"/>
+      <c r="Y5" s="107"/>
+      <c r="Z5" s="107"/>
+      <c r="AA5" s="107"/>
+      <c r="AB5" s="107"/>
+      <c r="AC5" s="107"/>
+      <c r="AD5" s="107"/>
+      <c r="AE5" s="107"/>
+      <c r="AF5" s="107"/>
+      <c r="AG5" s="107"/>
+      <c r="AH5" s="107"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="119" t="s">
+      <c r="D7" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="121" t="s">
+      <c r="F7" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="113" t="s">
+      <c r="G7" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="114"/>
-      <c r="I7" s="94" t="s">
+      <c r="H7" s="111"/>
+      <c r="I7" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="95"/>
+      <c r="J7" s="123"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="115" t="s">
+      <c r="L7" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="116"/>
-      <c r="N7" s="115" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="116"/>
-      <c r="P7" s="103" t="s">
+      <c r="M7" s="113"/>
+      <c r="N7" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="113"/>
+      <c r="P7" s="126" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="17"/>
-      <c r="R7" s="96" t="s">
+      <c r="R7" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="97"/>
+      <c r="S7" s="115"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="96" t="s">
+      <c r="U7" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="97"/>
-      <c r="W7" s="96" t="s">
+      <c r="V7" s="115"/>
+      <c r="W7" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="96" t="s">
+      <c r="X7" s="115"/>
+      <c r="Y7" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="96" t="s">
+      <c r="Z7" s="115"/>
+      <c r="AA7" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="97"/>
-      <c r="AC7" s="96" t="s">
+      <c r="AB7" s="115"/>
+      <c r="AC7" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="97"/>
-      <c r="AE7" s="96" t="s">
+      <c r="AD7" s="115"/>
+      <c r="AE7" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="97"/>
+      <c r="AF7" s="115"/>
       <c r="AG7" s="13"/>
-      <c r="AH7" s="105" t="s">
+      <c r="AH7" s="128" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="102"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="122"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="121"/>
       <c r="G8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="O8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="104"/>
+      <c r="P8" s="127"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="25" t="s">
         <v>9</v>
@@ -2506,7 +2506,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="16"/>
-      <c r="AH8" s="106"/>
+      <c r="AH8" s="129"/>
     </row>
     <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
@@ -4510,46 +4510,46 @@
       <c r="AH28" s="5"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="98" t="s">
+      <c r="C29" s="105"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="100"/>
-      <c r="G29" s="98" t="s">
+      <c r="F29" s="106"/>
+      <c r="G29" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="99"/>
-      <c r="N29" s="99"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="100"/>
-      <c r="R29" s="98" t="s">
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="106"/>
+      <c r="R29" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="99"/>
-      <c r="T29" s="99"/>
-      <c r="U29" s="99"/>
-      <c r="V29" s="99"/>
-      <c r="W29" s="99"/>
-      <c r="X29" s="99"/>
-      <c r="Y29" s="99"/>
-      <c r="Z29" s="99"/>
-      <c r="AA29" s="99"/>
-      <c r="AB29" s="99"/>
-      <c r="AC29" s="99"/>
-      <c r="AD29" s="99"/>
-      <c r="AE29" s="99"/>
-      <c r="AF29" s="99"/>
-      <c r="AG29" s="99"/>
-      <c r="AH29" s="100"/>
+      <c r="S29" s="105"/>
+      <c r="T29" s="105"/>
+      <c r="U29" s="105"/>
+      <c r="V29" s="105"/>
+      <c r="W29" s="105"/>
+      <c r="X29" s="105"/>
+      <c r="Y29" s="105"/>
+      <c r="Z29" s="105"/>
+      <c r="AA29" s="105"/>
+      <c r="AB29" s="105"/>
+      <c r="AC29" s="105"/>
+      <c r="AD29" s="105"/>
+      <c r="AE29" s="105"/>
+      <c r="AF29" s="105"/>
+      <c r="AG29" s="105"/>
+      <c r="AH29" s="106"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="10"/>
@@ -4928,6 +4928,16 @@
     <sortCondition ref="AL9"/>
   </sortState>
   <mergeCells count="26">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AH7:AH8"/>
     <mergeCell ref="B2:AH2"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
@@ -4944,16 +4954,6 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="U7:V7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="R29:AH29"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AH7:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -4968,8 +4968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5005,76 +5005,76 @@
     </row>
     <row r="4" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="L5" s="128" t="s">
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="L5" s="132" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="128"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="128"/>
-      <c r="P5" s="128"/>
-      <c r="R5" s="129" t="s">
+      <c r="M5" s="132"/>
+      <c r="N5" s="132"/>
+      <c r="O5" s="132"/>
+      <c r="P5" s="132"/>
+      <c r="R5" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="129"/>
-      <c r="T5" s="129"/>
-      <c r="U5" s="129"/>
-      <c r="V5" s="129"/>
-      <c r="W5" s="129"/>
-      <c r="X5" s="129"/>
-      <c r="Y5" s="129"/>
-      <c r="Z5" s="129"/>
-      <c r="AA5" s="129"/>
-      <c r="AB5" s="129"/>
-      <c r="AC5" s="129"/>
-      <c r="AD5" s="129"/>
-      <c r="AE5" s="129"/>
-      <c r="AF5" s="129"/>
-      <c r="AG5" s="129"/>
-      <c r="AH5" s="129"/>
+      <c r="S5" s="133"/>
+      <c r="T5" s="133"/>
+      <c r="U5" s="133"/>
+      <c r="V5" s="133"/>
+      <c r="W5" s="133"/>
+      <c r="X5" s="133"/>
+      <c r="Y5" s="133"/>
+      <c r="Z5" s="133"/>
+      <c r="AA5" s="133"/>
+      <c r="AB5" s="133"/>
+      <c r="AC5" s="133"/>
+      <c r="AD5" s="133"/>
+      <c r="AE5" s="133"/>
+      <c r="AF5" s="133"/>
+      <c r="AG5" s="133"/>
+      <c r="AH5" s="133"/>
     </row>
     <row r="6" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="128"/>
-      <c r="P6" s="128"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129"/>
-      <c r="X6" s="129"/>
-      <c r="Y6" s="129"/>
-      <c r="Z6" s="129"/>
-      <c r="AA6" s="129"/>
-      <c r="AB6" s="129"/>
-      <c r="AC6" s="129"/>
-      <c r="AD6" s="129"/>
-      <c r="AE6" s="129"/>
-      <c r="AF6" s="129"/>
-      <c r="AG6" s="129"/>
-      <c r="AH6" s="129"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="R6" s="133"/>
+      <c r="S6" s="133"/>
+      <c r="T6" s="133"/>
+      <c r="U6" s="133"/>
+      <c r="V6" s="133"/>
+      <c r="W6" s="133"/>
+      <c r="X6" s="133"/>
+      <c r="Y6" s="133"/>
+      <c r="Z6" s="133"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="133"/>
+      <c r="AC6" s="133"/>
+      <c r="AD6" s="133"/>
+      <c r="AE6" s="133"/>
+      <c r="AF6" s="133"/>
+      <c r="AG6" s="133"/>
+      <c r="AH6" s="133"/>
     </row>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="134" t="s">
@@ -5086,10 +5086,10 @@
       <c r="D7" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="135" t="s">
+      <c r="E7" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="138" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="130" t="s">
@@ -5135,11 +5135,11 @@
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="132"/>
+      <c r="B8" s="135"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="139"/>
       <c r="G8" s="92" t="s">
         <v>9</v>
       </c>
@@ -5168,20 +5168,23 @@
       <c r="AH8" s="93"/>
     </row>
     <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="137" t="s">
+      <c r="B9" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="C9" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="141">
+      <c r="D9" s="98">
         <v>38226</v>
       </c>
-      <c r="E9" s="143">
+      <c r="E9" s="100">
         <f ca="1">(TODAY()-D9)/365</f>
-        <v>18.265753424657536</v>
-      </c>
-      <c r="F9" s="140"/>
+        <v>18.284931506849315</v>
+      </c>
+      <c r="F9" s="97">
+        <f ca="1">ROUNDDOWN(E9/5,0) + 2</f>
+        <v>5</v>
+      </c>
       <c r="G9" s="92">
         <v>21.68</v>
       </c>
@@ -5214,20 +5217,23 @@
       </c>
     </row>
     <row r="10" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="138" t="s">
+      <c r="C10" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="142">
+      <c r="D10" s="99">
         <v>37601</v>
       </c>
-      <c r="E10" s="143">
+      <c r="E10" s="100">
         <f t="shared" ref="E10:E25" ca="1" si="0">(TODAY()-D10)/365</f>
-        <v>19.978082191780821</v>
-      </c>
-      <c r="F10" s="139"/>
+        <v>19.997260273972604</v>
+      </c>
+      <c r="F10" s="97">
+        <f t="shared" ref="F10:F25" ca="1" si="1">ROUNDDOWN(E10/5,0) + 2</f>
+        <v>5</v>
+      </c>
       <c r="G10" s="92">
         <v>23.05</v>
       </c>
@@ -5260,20 +5266,23 @@
       </c>
     </row>
     <row r="11" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="138" t="s">
+      <c r="C11" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="142">
+      <c r="D11" s="99">
         <v>35826</v>
       </c>
-      <c r="E11" s="143">
+      <c r="E11" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>24.841095890410958</v>
-      </c>
-      <c r="F11" s="139"/>
+        <v>24.860273972602741</v>
+      </c>
+      <c r="F11" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
       <c r="G11" s="92">
         <v>26.94</v>
       </c>
@@ -5306,20 +5315,23 @@
       </c>
     </row>
     <row r="12" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="142">
+      <c r="D12" s="99">
         <v>35403</v>
       </c>
-      <c r="E12" s="143">
+      <c r="E12" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="F12" s="139"/>
+        <v>26.019178082191782</v>
+      </c>
+      <c r="F12" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
       <c r="G12" s="92">
         <v>27.87</v>
       </c>
@@ -5352,20 +5364,23 @@
       </c>
     </row>
     <row r="13" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="138" t="s">
+      <c r="B13" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="138" t="s">
+      <c r="C13" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="142">
+      <c r="D13" s="99">
         <v>33093</v>
       </c>
-      <c r="E13" s="143">
+      <c r="E13" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>32.328767123287669</v>
-      </c>
-      <c r="F13" s="139"/>
+        <v>32.347945205479455</v>
+      </c>
+      <c r="F13" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
       <c r="G13" s="92">
         <v>32.93</v>
       </c>
@@ -5398,20 +5413,23 @@
       </c>
     </row>
     <row r="14" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="142">
+      <c r="D14" s="99">
         <v>37900</v>
       </c>
-      <c r="E14" s="143">
+      <c r="E14" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>19.158904109589042</v>
-      </c>
-      <c r="F14" s="139"/>
+        <v>19.17808219178082</v>
+      </c>
+      <c r="F14" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
       <c r="G14" s="92">
         <v>22.4</v>
       </c>
@@ -5444,20 +5462,23 @@
       </c>
     </row>
     <row r="15" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="138" t="s">
+      <c r="C15" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="142">
+      <c r="D15" s="99">
         <v>35590</v>
       </c>
-      <c r="E15" s="143">
+      <c r="E15" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>25.487671232876714</v>
-      </c>
-      <c r="F15" s="139"/>
+        <v>25.506849315068493</v>
+      </c>
+      <c r="F15" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
       <c r="G15" s="92">
         <v>27.46</v>
       </c>
@@ -5490,20 +5511,23 @@
       </c>
     </row>
     <row r="16" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="142">
+      <c r="D16" s="99">
         <v>35192</v>
       </c>
-      <c r="E16" s="143">
+      <c r="E16" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>26.578082191780823</v>
-      </c>
-      <c r="F16" s="139"/>
+        <v>26.597260273972601</v>
+      </c>
+      <c r="F16" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
       <c r="G16" s="92">
         <v>28.33</v>
       </c>
@@ -5536,20 +5560,23 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="138" t="s">
+      <c r="B17" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="138" t="s">
+      <c r="C17" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="142">
+      <c r="D17" s="99">
         <v>36628</v>
       </c>
-      <c r="E17" s="143">
+      <c r="E17" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>22.643835616438356</v>
-      </c>
-      <c r="F17" s="139"/>
+        <v>22.663013698630138</v>
+      </c>
+      <c r="F17" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
       <c r="G17" s="92">
         <v>25.19</v>
       </c>
@@ -5582,20 +5609,23 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="138" t="s">
+      <c r="B18" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="138" t="s">
+      <c r="C18" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="142">
+      <c r="D18" s="99">
         <v>30115</v>
       </c>
-      <c r="E18" s="143">
+      <c r="E18" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>40.487671232876714</v>
-      </c>
-      <c r="F18" s="139"/>
+        <v>40.506849315068493</v>
+      </c>
+      <c r="F18" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
       <c r="G18" s="92">
         <v>39.46</v>
       </c>
@@ -5628,20 +5658,23 @@
       </c>
     </row>
     <row r="19" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="138" t="s">
+      <c r="B19" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="138" t="s">
+      <c r="C19" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="142">
+      <c r="D19" s="99">
         <v>41231</v>
       </c>
-      <c r="E19" s="143">
+      <c r="E19" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>10.032876712328767</v>
-      </c>
-      <c r="F19" s="139"/>
+        <v>10.052054794520547</v>
+      </c>
+      <c r="F19" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
       <c r="G19" s="92">
         <v>15.1</v>
       </c>
@@ -5674,20 +5707,23 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="138" t="s">
+      <c r="B20" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="138" t="s">
+      <c r="C20" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="142">
+      <c r="D20" s="99">
         <v>31824</v>
       </c>
-      <c r="E20" s="143">
+      <c r="E20" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>35.805479452054797</v>
-      </c>
-      <c r="F20" s="139"/>
+        <v>35.824657534246576</v>
+      </c>
+      <c r="F20" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
       <c r="G20" s="92">
         <v>35.71</v>
       </c>
@@ -5720,20 +5756,23 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="138" t="s">
+      <c r="C21" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="142">
+      <c r="D21" s="99">
         <v>38150</v>
       </c>
-      <c r="E21" s="143">
+      <c r="E21" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>18.473972602739725</v>
-      </c>
-      <c r="F21" s="139"/>
+        <v>18.493150684931507</v>
+      </c>
+      <c r="F21" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
       <c r="G21" s="92">
         <v>21.85</v>
       </c>
@@ -5766,20 +5805,23 @@
       </c>
     </row>
     <row r="22" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="138" t="s">
+      <c r="C22" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="142">
+      <c r="D22" s="99">
         <v>32891</v>
       </c>
-      <c r="E22" s="143">
+      <c r="E22" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>32.88219178082192</v>
-      </c>
-      <c r="F22" s="139"/>
+        <v>32.901369863013699</v>
+      </c>
+      <c r="F22" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
       <c r="G22" s="92">
         <v>33.380000000000003</v>
       </c>
@@ -5812,20 +5854,23 @@
       </c>
     </row>
     <row r="23" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="138" t="s">
+      <c r="B23" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="138" t="s">
+      <c r="C23" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="142">
+      <c r="D23" s="99">
         <v>41102</v>
       </c>
-      <c r="E23" s="143">
+      <c r="E23" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>10.386301369863014</v>
-      </c>
-      <c r="F23" s="139"/>
+        <v>10.405479452054795</v>
+      </c>
+      <c r="F23" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
       <c r="G23" s="92">
         <v>15.38</v>
       </c>
@@ -5858,20 +5903,23 @@
       </c>
     </row>
     <row r="24" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="139" t="s">
+      <c r="B24" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="139" t="s">
+      <c r="C24" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="142">
+      <c r="D24" s="99">
         <v>29465</v>
       </c>
-      <c r="E24" s="143">
+      <c r="E24" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>42.268493150684932</v>
-      </c>
-      <c r="F24" s="139"/>
+        <v>42.287671232876711</v>
+      </c>
+      <c r="F24" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
       <c r="G24" s="92">
         <v>40.880000000000003</v>
       </c>
@@ -5904,20 +5952,23 @@
       </c>
     </row>
     <row r="25" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="139" t="s">
+      <c r="C25" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="142">
+      <c r="D25" s="99">
         <v>30711</v>
       </c>
-      <c r="E25" s="143">
+      <c r="E25" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>38.854794520547948</v>
-      </c>
-      <c r="F25" s="139"/>
+        <v>38.873972602739727</v>
+      </c>
+      <c r="F25" s="97">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
       <c r="G25" s="92">
         <v>38.15</v>
       </c>
@@ -5985,7 +6036,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E9:E25" unlockedFormula="1"/>
+    <ignoredError sqref="E9:E25 F9:F25" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6010,15 +6061,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="140" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="124" t="s">
+      <c r="C4" s="141" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="88" t="s">
@@ -6026,25 +6077,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="125"/>
+      <c r="C5" s="142"/>
       <c r="D5" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="125"/>
+      <c r="C6" s="142"/>
       <c r="D6" s="71" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="125"/>
+      <c r="C7" s="142"/>
       <c r="D7" s="70" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="126"/>
+      <c r="C8" s="143"/>
       <c r="D8" s="89" t="s">
         <v>56</v>
       </c>
@@ -6064,7 +6115,7 @@
       <c r="C11" s="72"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="141" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="88" t="s">
@@ -6072,43 +6123,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="125"/>
+      <c r="C13" s="142"/>
       <c r="D13" s="70" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="125"/>
+      <c r="C14" s="142"/>
       <c r="D14" s="68" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="125"/>
+      <c r="C15" s="142"/>
       <c r="D15" s="87" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="125"/>
+      <c r="C16" s="142"/>
       <c r="D16" s="68" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="125"/>
+      <c r="C17" s="142"/>
       <c r="D17" s="87" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="125"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="68" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="126"/>
+      <c r="C19" s="143"/>
       <c r="D19" s="89" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
mise en forme tableaux et debut des formules de primes
</commit_message>
<xml_diff>
--- a/EE04.xlsx
+++ b/EE04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olimo\remise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EC7682-01A6-4602-99E1-7571CD1AAC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0737FE4C-A04E-4C03-9A3A-C155594BCFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="72">
   <si>
     <t>Ventes réalisées</t>
   </si>
@@ -574,17 +574,28 @@
       <t>S</t>
     </r>
   </si>
+  <si>
+    <t>Horaire reg.</t>
+  </si>
+  <si>
+    <t>Égibilité</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -737,6 +748,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -848,7 +888,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1320,26 +1360,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -1363,11 +1383,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1699,211 +1780,358 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2246,7 +2474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH55"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
@@ -2274,41 +2502,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="19.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="101"/>
-      <c r="W2" s="101"/>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="101"/>
-      <c r="Z2" s="101"/>
-      <c r="AA2" s="101"/>
-      <c r="AB2" s="101"/>
-      <c r="AC2" s="101"/>
-      <c r="AD2" s="101"/>
-      <c r="AE2" s="101"/>
-      <c r="AF2" s="101"/>
-      <c r="AG2" s="101"/>
-      <c r="AH2" s="101"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
+      <c r="AA2" s="97"/>
+      <c r="AB2" s="97"/>
+      <c r="AC2" s="97"/>
+      <c r="AD2" s="97"/>
+      <c r="AE2" s="97"/>
+      <c r="AF2" s="97"/>
+      <c r="AG2" s="97"/>
+      <c r="AH2" s="97"/>
     </row>
     <row r="3" spans="2:34" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -2319,122 +2547,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="L5" s="103" t="s">
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="L5" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="R5" s="107" t="s">
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="R5" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
-      <c r="AC5" s="107"/>
-      <c r="AD5" s="107"/>
-      <c r="AE5" s="107"/>
-      <c r="AF5" s="107"/>
-      <c r="AG5" s="107"/>
-      <c r="AH5" s="107"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
+      <c r="Z5" s="103"/>
+      <c r="AA5" s="103"/>
+      <c r="AB5" s="103"/>
+      <c r="AC5" s="103"/>
+      <c r="AD5" s="103"/>
+      <c r="AE5" s="103"/>
+      <c r="AF5" s="103"/>
+      <c r="AG5" s="103"/>
+      <c r="AH5" s="103"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="D7" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="120" t="s">
+      <c r="F7" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="110" t="s">
+      <c r="G7" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="111"/>
-      <c r="I7" s="122" t="s">
+      <c r="H7" s="107"/>
+      <c r="I7" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="123"/>
+      <c r="J7" s="119"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="112" t="s">
+      <c r="L7" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="113"/>
-      <c r="N7" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="113"/>
-      <c r="P7" s="126" t="s">
+      <c r="M7" s="109"/>
+      <c r="N7" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="109"/>
+      <c r="P7" s="122" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="17"/>
-      <c r="R7" s="114" t="s">
+      <c r="R7" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="115"/>
+      <c r="S7" s="111"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="114" t="s">
+      <c r="U7" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="115"/>
-      <c r="W7" s="114" t="s">
+      <c r="V7" s="111"/>
+      <c r="W7" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="115"/>
-      <c r="Y7" s="114" t="s">
+      <c r="X7" s="111"/>
+      <c r="Y7" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="115"/>
-      <c r="AA7" s="114" t="s">
+      <c r="Z7" s="111"/>
+      <c r="AA7" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="115"/>
-      <c r="AC7" s="114" t="s">
+      <c r="AB7" s="111"/>
+      <c r="AC7" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="115"/>
-      <c r="AE7" s="114" t="s">
+      <c r="AD7" s="111"/>
+      <c r="AE7" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="115"/>
+      <c r="AF7" s="111"/>
       <c r="AG7" s="13"/>
-      <c r="AH7" s="128" t="s">
+      <c r="AH7" s="124" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="125"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="121"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="117"/>
       <c r="G8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2460,7 +2688,7 @@
       <c r="O8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="127"/>
+      <c r="P8" s="123"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="25" t="s">
         <v>9</v>
@@ -2506,7 +2734,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="16"/>
-      <c r="AH8" s="129"/>
+      <c r="AH8" s="125"/>
     </row>
     <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
@@ -4510,46 +4738,46 @@
       <c r="AH28" s="5"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="104" t="s">
+      <c r="B29" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="104" t="s">
+      <c r="C29" s="101"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="106"/>
-      <c r="G29" s="104" t="s">
+      <c r="F29" s="102"/>
+      <c r="G29" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="105"/>
-      <c r="P29" s="106"/>
-      <c r="R29" s="104" t="s">
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="101"/>
+      <c r="P29" s="102"/>
+      <c r="R29" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="105"/>
-      <c r="T29" s="105"/>
-      <c r="U29" s="105"/>
-      <c r="V29" s="105"/>
-      <c r="W29" s="105"/>
-      <c r="X29" s="105"/>
-      <c r="Y29" s="105"/>
-      <c r="Z29" s="105"/>
-      <c r="AA29" s="105"/>
-      <c r="AB29" s="105"/>
-      <c r="AC29" s="105"/>
-      <c r="AD29" s="105"/>
-      <c r="AE29" s="105"/>
-      <c r="AF29" s="105"/>
-      <c r="AG29" s="105"/>
-      <c r="AH29" s="106"/>
+      <c r="S29" s="101"/>
+      <c r="T29" s="101"/>
+      <c r="U29" s="101"/>
+      <c r="V29" s="101"/>
+      <c r="W29" s="101"/>
+      <c r="X29" s="101"/>
+      <c r="Y29" s="101"/>
+      <c r="Z29" s="101"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="101"/>
+      <c r="AC29" s="101"/>
+      <c r="AD29" s="101"/>
+      <c r="AE29" s="101"/>
+      <c r="AF29" s="101"/>
+      <c r="AG29" s="101"/>
+      <c r="AH29" s="102"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="10"/>
@@ -4968,8 +5196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7:AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4979,18 +5207,22 @@
     <col min="3" max="3" width="4.42578125" style="92" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="92" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="92" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="92" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="92" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="92"/>
-    <col min="9" max="9" width="23.42578125" style="92" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="92" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="92"/>
+    <col min="9" max="10" width="13.42578125" style="92" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="92" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" style="92" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="92"/>
     <col min="14" max="14" width="13.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="92" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="92" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.7109375" style="92"/>
+    <col min="17" max="17" width="10.7109375" style="92"/>
+    <col min="18" max="18" width="11" style="92" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" style="92" customWidth="1"/>
+    <col min="20" max="33" width="10.7109375" style="92"/>
+    <col min="34" max="34" width="13.85546875" style="92" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="10.7109375" style="92"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5005,1005 +5237,1515 @@
     </row>
     <row r="4" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="L5" s="132" t="s">
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="L5" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="132"/>
-      <c r="N5" s="132"/>
-      <c r="O5" s="132"/>
-      <c r="P5" s="132"/>
-      <c r="R5" s="133" t="s">
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="R5" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="133"/>
-      <c r="T5" s="133"/>
-      <c r="U5" s="133"/>
-      <c r="V5" s="133"/>
-      <c r="W5" s="133"/>
-      <c r="X5" s="133"/>
-      <c r="Y5" s="133"/>
-      <c r="Z5" s="133"/>
-      <c r="AA5" s="133"/>
-      <c r="AB5" s="133"/>
-      <c r="AC5" s="133"/>
-      <c r="AD5" s="133"/>
-      <c r="AE5" s="133"/>
-      <c r="AF5" s="133"/>
-      <c r="AG5" s="133"/>
-      <c r="AH5" s="133"/>
+      <c r="S5" s="128"/>
+      <c r="T5" s="128"/>
+      <c r="U5" s="128"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="128"/>
+      <c r="Z5" s="128"/>
+      <c r="AA5" s="128"/>
+      <c r="AB5" s="128"/>
+      <c r="AC5" s="128"/>
+      <c r="AD5" s="128"/>
+      <c r="AE5" s="128"/>
+      <c r="AF5" s="128"/>
+      <c r="AG5" s="128"/>
+      <c r="AH5" s="128"/>
     </row>
     <row r="6" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="132"/>
-      <c r="P6" s="132"/>
-      <c r="R6" s="133"/>
-      <c r="S6" s="133"/>
-      <c r="T6" s="133"/>
-      <c r="U6" s="133"/>
-      <c r="V6" s="133"/>
-      <c r="W6" s="133"/>
-      <c r="X6" s="133"/>
-      <c r="Y6" s="133"/>
-      <c r="Z6" s="133"/>
-      <c r="AA6" s="133"/>
-      <c r="AB6" s="133"/>
-      <c r="AC6" s="133"/>
-      <c r="AD6" s="133"/>
-      <c r="AE6" s="133"/>
-      <c r="AF6" s="133"/>
-      <c r="AG6" s="133"/>
-      <c r="AH6" s="133"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="128"/>
+      <c r="T6" s="128"/>
+      <c r="U6" s="128"/>
+      <c r="V6" s="128"/>
+      <c r="W6" s="128"/>
+      <c r="X6" s="128"/>
+      <c r="Y6" s="128"/>
+      <c r="Z6" s="128"/>
+      <c r="AA6" s="128"/>
+      <c r="AB6" s="128"/>
+      <c r="AC6" s="128"/>
+      <c r="AD6" s="128"/>
+      <c r="AE6" s="128"/>
+      <c r="AF6" s="128"/>
+      <c r="AG6" s="128"/>
+      <c r="AH6" s="128"/>
     </row>
     <row r="7" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="134" t="s">
+      <c r="C7" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="134" t="s">
+      <c r="D7" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="136" t="s">
+      <c r="E7" s="148" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="138" t="s">
+      <c r="F7" s="148" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="130" t="s">
+      <c r="G7" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130" t="s">
+      <c r="H7" s="147"/>
+      <c r="I7" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="130"/>
-      <c r="L7" s="92" t="s">
+      <c r="J7" s="147"/>
+      <c r="L7" s="155" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="93" t="s">
+      <c r="M7" s="160"/>
+      <c r="N7" s="161" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="160"/>
+      <c r="P7" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="92" t="s">
+      <c r="R7" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="92" t="s">
+      <c r="S7" s="166"/>
+      <c r="T7" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="W7" s="92" t="s">
+      <c r="U7" s="166"/>
+      <c r="V7" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="Y7" s="92" t="s">
+      <c r="W7" s="166"/>
+      <c r="X7" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" s="92" t="s">
+      <c r="Y7" s="166"/>
+      <c r="Z7" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="AC7" s="92" t="s">
+      <c r="AA7" s="166"/>
+      <c r="AB7" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="AE7" s="92" t="s">
+      <c r="AC7" s="166"/>
+      <c r="AD7" s="167" t="s">
         <v>46</v>
       </c>
+      <c r="AE7" s="166"/>
       <c r="AH7" s="93" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="135"/>
-      <c r="C8" s="135"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="92" t="s">
+      <c r="B8" s="137"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="148"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="92" t="s">
+      <c r="H8" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="92" t="s">
+      <c r="I8" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="92" t="s">
+      <c r="J8" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="92" t="s">
+      <c r="L8" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="92" t="s">
+      <c r="M8" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="92" t="s">
+      <c r="N8" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="92" t="s">
+      <c r="O8" s="158" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="93"/>
+      <c r="P8" s="138"/>
+      <c r="R8" s="162" t="s">
+        <v>69</v>
+      </c>
+      <c r="S8" s="164" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="157" t="s">
+        <v>70</v>
+      </c>
+      <c r="U8" s="159" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" s="159" t="s">
+        <v>70</v>
+      </c>
+      <c r="W8" s="159" t="s">
+        <v>40</v>
+      </c>
+      <c r="X8" s="159" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="159" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z8" s="159" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA8" s="159" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB8" s="159" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC8" s="159" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD8" s="159" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE8" s="159" t="s">
+        <v>40</v>
+      </c>
       <c r="AH8" s="93"/>
     </row>
-    <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="141" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="98">
+      <c r="D9" s="144">
         <v>38226</v>
       </c>
-      <c r="E9" s="100">
+      <c r="E9" s="152">
         <f ca="1">(TODAY()-D9)/365</f>
         <v>18.284931506849315</v>
       </c>
-      <c r="F9" s="97">
+      <c r="F9" s="153">
         <f ca="1">ROUNDDOWN(E9/5,0) + 2</f>
         <v>5</v>
       </c>
-      <c r="G9" s="92">
+      <c r="G9" s="145">
         <v>21.68</v>
       </c>
-      <c r="H9" s="92">
+      <c r="H9" s="146">
         <v>32.520000000000003</v>
       </c>
-      <c r="I9" s="92">
+      <c r="I9" s="146">
         <v>86639.77</v>
       </c>
-      <c r="J9" s="92">
+      <c r="J9" s="133">
         <v>138605.66</v>
       </c>
-      <c r="K9" s="92">
-        <v>0</v>
-      </c>
-      <c r="L9" s="92">
+      <c r="L9" s="157">
         <v>1837.5</v>
       </c>
-      <c r="M9" s="92">
+      <c r="M9" s="159">
         <v>12.7</v>
       </c>
-      <c r="N9" s="92">
+      <c r="N9" s="145">
         <v>87225.33</v>
       </c>
-      <c r="O9" s="92">
+      <c r="O9" s="146">
         <v>113521.61</v>
       </c>
       <c r="P9" s="92">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="163">
+        <f>G9*L9</f>
+        <v>39837</v>
+      </c>
+      <c r="S9" s="165">
+        <f>H9*M9</f>
+        <v>413.00400000000002</v>
+      </c>
+      <c r="T9" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9" s="165">
+        <f>(0.01*N9)+(0.015*O9)</f>
+        <v>2575.0774499999998</v>
+      </c>
+      <c r="V9" s="159"/>
+      <c r="W9" s="159"/>
+      <c r="X9" s="159"/>
+      <c r="Y9" s="159"/>
+      <c r="Z9" s="159"/>
+      <c r="AA9" s="159"/>
+      <c r="AB9" s="157"/>
+      <c r="AC9" s="159"/>
+      <c r="AD9" s="159"/>
+      <c r="AE9" s="159"/>
+      <c r="AH9" s="135">
+        <f>SUM(R9:AE9)</f>
+        <v>42825.081449999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="99">
+      <c r="D10" s="144">
         <v>37601</v>
       </c>
-      <c r="E10" s="100">
+      <c r="E10" s="152">
         <f t="shared" ref="E10:E25" ca="1" si="0">(TODAY()-D10)/365</f>
         <v>19.997260273972604</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="153">
         <f t="shared" ref="F10:F25" ca="1" si="1">ROUNDDOWN(E10/5,0) + 2</f>
         <v>5</v>
       </c>
-      <c r="G10" s="92">
+      <c r="G10" s="145">
         <v>23.05</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="146">
         <v>34.58</v>
       </c>
-      <c r="I10" s="92">
+      <c r="I10" s="146">
         <v>86104.49</v>
       </c>
-      <c r="J10" s="92">
+      <c r="J10" s="133">
         <v>141119.44</v>
       </c>
-      <c r="K10" s="92">
-        <v>0</v>
-      </c>
-      <c r="L10" s="92">
+      <c r="L10" s="157">
         <v>1800</v>
       </c>
-      <c r="M10" s="92">
+      <c r="M10" s="159">
         <v>25.2</v>
       </c>
-      <c r="N10" s="92">
+      <c r="N10" s="145">
         <v>100494.47</v>
       </c>
-      <c r="O10" s="92">
+      <c r="O10" s="146">
         <v>133202.71</v>
       </c>
       <c r="P10" s="92">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="163">
+        <f t="shared" ref="R10:R25" si="2">G10*L10</f>
+        <v>41490</v>
+      </c>
+      <c r="S10" s="165">
+        <f t="shared" ref="S10:S25" si="3">H10*M10</f>
+        <v>871.41599999999994</v>
+      </c>
+      <c r="T10" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U10" s="165">
+        <f t="shared" ref="U10:U25" si="4">(0.01*N10)+(0.015*O10)</f>
+        <v>3002.9853499999999</v>
+      </c>
+      <c r="V10" s="159"/>
+      <c r="W10" s="159"/>
+      <c r="X10" s="159"/>
+      <c r="Y10" s="159"/>
+      <c r="Z10" s="159"/>
+      <c r="AA10" s="159"/>
+      <c r="AB10" s="157"/>
+      <c r="AC10" s="159"/>
+      <c r="AD10" s="159"/>
+      <c r="AE10" s="159"/>
+      <c r="AH10" s="135">
+        <f t="shared" ref="AH10:AH25" si="5">SUM(R10:AE10)</f>
+        <v>45364.40135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="99">
+      <c r="D11" s="144">
         <v>35826</v>
       </c>
-      <c r="E11" s="100">
+      <c r="E11" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>24.860273972602741</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="G11" s="92">
+      <c r="G11" s="145">
         <v>26.94</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="146">
         <v>40.409999999999997</v>
       </c>
-      <c r="I11" s="92">
+      <c r="I11" s="146">
         <v>89605.86</v>
       </c>
-      <c r="J11" s="92">
+      <c r="J11" s="133">
         <v>156292.04</v>
       </c>
-      <c r="K11" s="92">
-        <v>0</v>
-      </c>
-      <c r="L11" s="92">
+      <c r="L11" s="157">
         <v>1800</v>
       </c>
-      <c r="M11" s="92">
-        <v>0</v>
-      </c>
-      <c r="N11" s="92">
+      <c r="M11" s="159">
+        <v>0</v>
+      </c>
+      <c r="N11" s="145">
         <v>76821.77</v>
       </c>
-      <c r="O11" s="92">
+      <c r="O11" s="146">
         <v>158727.13</v>
       </c>
       <c r="P11" s="92">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="163">
+        <f t="shared" si="2"/>
+        <v>48492</v>
+      </c>
+      <c r="S11" s="165">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U11" s="165">
+        <f t="shared" si="4"/>
+        <v>3149.1246500000002</v>
+      </c>
+      <c r="V11" s="159"/>
+      <c r="W11" s="159"/>
+      <c r="X11" s="159"/>
+      <c r="Y11" s="159"/>
+      <c r="Z11" s="159"/>
+      <c r="AA11" s="159"/>
+      <c r="AB11" s="157"/>
+      <c r="AC11" s="159"/>
+      <c r="AD11" s="159"/>
+      <c r="AE11" s="159"/>
+      <c r="AH11" s="135">
+        <f t="shared" si="5"/>
+        <v>51641.124649999998</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="99">
+      <c r="D12" s="144">
         <v>35403</v>
       </c>
-      <c r="E12" s="100">
+      <c r="E12" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>26.019178082191782</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F12" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="G12" s="92">
+      <c r="G12" s="145">
         <v>27.87</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="146">
         <v>41.81</v>
       </c>
-      <c r="I12" s="92">
+      <c r="I12" s="146">
         <v>88556.09</v>
       </c>
-      <c r="J12" s="92">
+      <c r="J12" s="133">
         <v>156576.41</v>
       </c>
-      <c r="K12" s="92">
-        <v>0</v>
-      </c>
-      <c r="L12" s="92">
+      <c r="L12" s="157">
         <v>1762.5</v>
       </c>
-      <c r="M12" s="92">
-        <v>0</v>
-      </c>
-      <c r="N12" s="92">
+      <c r="M12" s="159">
+        <v>0</v>
+      </c>
+      <c r="N12" s="145">
         <v>77813.539999999994</v>
       </c>
-      <c r="O12" s="92">
+      <c r="O12" s="146">
         <v>170576.59</v>
       </c>
       <c r="P12" s="92">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="163">
+        <f t="shared" si="2"/>
+        <v>49120.875</v>
+      </c>
+      <c r="S12" s="165">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U12" s="165">
+        <f t="shared" si="4"/>
+        <v>3336.7842500000002</v>
+      </c>
+      <c r="V12" s="159"/>
+      <c r="W12" s="159"/>
+      <c r="X12" s="159"/>
+      <c r="Y12" s="159"/>
+      <c r="Z12" s="159"/>
+      <c r="AA12" s="159"/>
+      <c r="AB12" s="157"/>
+      <c r="AC12" s="159"/>
+      <c r="AD12" s="159"/>
+      <c r="AE12" s="159"/>
+      <c r="AH12" s="135">
+        <f t="shared" si="5"/>
+        <v>52457.659249999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="99">
+      <c r="D13" s="144">
         <v>33093</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>32.347945205479455</v>
       </c>
-      <c r="F13" s="97">
+      <c r="F13" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
-      <c r="G13" s="92">
+      <c r="G13" s="145">
         <v>32.93</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="146">
         <v>49.4</v>
       </c>
-      <c r="I13" s="92">
+      <c r="I13" s="146">
         <v>91038.77</v>
       </c>
-      <c r="J13" s="92">
+      <c r="J13" s="133">
         <v>172168.01</v>
       </c>
-      <c r="K13" s="92">
-        <v>0</v>
-      </c>
-      <c r="L13" s="92">
+      <c r="L13" s="157">
         <v>1725</v>
       </c>
-      <c r="M13" s="92">
+      <c r="M13" s="159">
         <v>39.57</v>
       </c>
-      <c r="N13" s="92">
+      <c r="N13" s="145">
         <v>96236.12</v>
       </c>
-      <c r="O13" s="92">
+      <c r="O13" s="146">
         <v>177509.88</v>
       </c>
       <c r="P13" s="92">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R13" s="163">
+        <f t="shared" si="2"/>
+        <v>56804.25</v>
+      </c>
+      <c r="S13" s="165">
+        <f t="shared" si="3"/>
+        <v>1954.758</v>
+      </c>
+      <c r="T13" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U13" s="165">
+        <f t="shared" si="4"/>
+        <v>3625.0093999999999</v>
+      </c>
+      <c r="V13" s="159"/>
+      <c r="W13" s="159"/>
+      <c r="X13" s="159"/>
+      <c r="Y13" s="159"/>
+      <c r="Z13" s="159"/>
+      <c r="AA13" s="159"/>
+      <c r="AB13" s="157"/>
+      <c r="AC13" s="159"/>
+      <c r="AD13" s="159"/>
+      <c r="AE13" s="159"/>
+      <c r="AH13" s="135">
+        <f t="shared" si="5"/>
+        <v>62384.017400000004</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="99">
+      <c r="D14" s="144">
         <v>37900</v>
       </c>
-      <c r="E14" s="100">
+      <c r="E14" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>19.17808219178082</v>
       </c>
-      <c r="F14" s="97">
+      <c r="F14" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="G14" s="92">
+      <c r="G14" s="145">
         <v>22.4</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="146">
         <v>33.6</v>
       </c>
-      <c r="I14" s="92">
+      <c r="I14" s="146">
         <v>87296.23</v>
       </c>
-      <c r="J14" s="92">
+      <c r="J14" s="133">
         <v>141450.34</v>
       </c>
-      <c r="K14" s="92">
-        <v>0</v>
-      </c>
-      <c r="L14" s="92">
+      <c r="L14" s="157">
         <v>1837.5</v>
       </c>
-      <c r="M14" s="92">
+      <c r="M14" s="159">
         <v>98.2</v>
       </c>
-      <c r="N14" s="92">
+      <c r="N14" s="145">
         <v>86363.33</v>
       </c>
-      <c r="O14" s="92">
+      <c r="O14" s="146">
         <v>120584.13</v>
       </c>
       <c r="P14" s="92">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="163">
+        <f t="shared" si="2"/>
+        <v>41160</v>
+      </c>
+      <c r="S14" s="165">
+        <f t="shared" si="3"/>
+        <v>3299.5200000000004</v>
+      </c>
+      <c r="T14" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U14" s="165">
+        <f t="shared" si="4"/>
+        <v>2672.39525</v>
+      </c>
+      <c r="V14" s="159"/>
+      <c r="W14" s="159"/>
+      <c r="X14" s="159"/>
+      <c r="Y14" s="159"/>
+      <c r="Z14" s="159"/>
+      <c r="AA14" s="159"/>
+      <c r="AB14" s="157"/>
+      <c r="AC14" s="159"/>
+      <c r="AD14" s="159"/>
+      <c r="AE14" s="159"/>
+      <c r="AH14" s="135">
+        <f t="shared" si="5"/>
+        <v>47131.915250000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="99">
+      <c r="D15" s="144">
         <v>35590</v>
       </c>
-      <c r="E15" s="100">
+      <c r="E15" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>25.506849315068493</v>
       </c>
-      <c r="F15" s="97">
+      <c r="F15" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="G15" s="92">
+      <c r="G15" s="145">
         <v>27.46</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="146">
         <v>41.19</v>
       </c>
-      <c r="I15" s="92">
+      <c r="I15" s="146">
         <v>88194.9</v>
       </c>
-      <c r="J15" s="92">
+      <c r="J15" s="133">
         <v>155011.24</v>
       </c>
-      <c r="K15" s="92">
-        <v>0</v>
-      </c>
-      <c r="L15" s="92">
+      <c r="L15" s="157">
         <v>1762.5</v>
       </c>
-      <c r="M15" s="92">
+      <c r="M15" s="159">
         <v>244.14</v>
       </c>
-      <c r="N15" s="92">
+      <c r="N15" s="145">
         <v>98812.43</v>
       </c>
-      <c r="O15" s="92">
+      <c r="O15" s="146">
         <v>119521.7</v>
       </c>
       <c r="P15" s="92">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:34" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R15" s="163">
+        <f t="shared" si="2"/>
+        <v>48398.25</v>
+      </c>
+      <c r="S15" s="165">
+        <f t="shared" si="3"/>
+        <v>10056.1266</v>
+      </c>
+      <c r="T15" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U15" s="165">
+        <f t="shared" si="4"/>
+        <v>2780.9497999999999</v>
+      </c>
+      <c r="V15" s="159"/>
+      <c r="W15" s="159"/>
+      <c r="X15" s="159"/>
+      <c r="Y15" s="159"/>
+      <c r="Z15" s="159"/>
+      <c r="AA15" s="159"/>
+      <c r="AB15" s="157"/>
+      <c r="AC15" s="159"/>
+      <c r="AD15" s="159"/>
+      <c r="AE15" s="159"/>
+      <c r="AH15" s="135">
+        <f t="shared" si="5"/>
+        <v>61235.326400000005</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="99">
+      <c r="D16" s="144">
         <v>35192</v>
       </c>
-      <c r="E16" s="100">
+      <c r="E16" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>26.597260273972601</v>
       </c>
-      <c r="F16" s="97">
+      <c r="F16" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="G16" s="92">
+      <c r="G16" s="145">
         <v>28.33</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="146">
         <v>42.5</v>
       </c>
-      <c r="I16" s="92">
+      <c r="I16" s="146">
         <v>88963.64</v>
       </c>
-      <c r="J16" s="92">
+      <c r="J16" s="133">
         <v>158342.45000000001</v>
       </c>
-      <c r="K16" s="92">
-        <v>0</v>
-      </c>
-      <c r="L16" s="92">
+      <c r="L16" s="157">
         <v>1762.5</v>
       </c>
-      <c r="M16" s="92">
+      <c r="M16" s="159">
         <v>109.39</v>
       </c>
-      <c r="N16" s="92">
+      <c r="N16" s="145">
         <v>89879.18</v>
       </c>
-      <c r="O16" s="92">
+      <c r="O16" s="146">
         <v>164850.17000000001</v>
       </c>
       <c r="P16" s="92">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R16" s="163">
+        <f t="shared" si="2"/>
+        <v>49931.625</v>
+      </c>
+      <c r="S16" s="165">
+        <f t="shared" si="3"/>
+        <v>4649.0749999999998</v>
+      </c>
+      <c r="T16" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U16" s="165">
+        <f t="shared" si="4"/>
+        <v>3371.5443500000001</v>
+      </c>
+      <c r="V16" s="159"/>
+      <c r="W16" s="159"/>
+      <c r="X16" s="159"/>
+      <c r="Y16" s="159"/>
+      <c r="Z16" s="159"/>
+      <c r="AA16" s="159"/>
+      <c r="AB16" s="157"/>
+      <c r="AC16" s="159"/>
+      <c r="AD16" s="159"/>
+      <c r="AE16" s="159"/>
+      <c r="AH16" s="135">
+        <f t="shared" si="5"/>
+        <v>57952.244349999994</v>
+      </c>
+    </row>
+    <row r="17" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="99">
+      <c r="D17" s="144">
         <v>36628</v>
       </c>
-      <c r="E17" s="100">
+      <c r="E17" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>22.663013698630138</v>
       </c>
-      <c r="F17" s="97">
+      <c r="F17" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="G17" s="92">
+      <c r="G17" s="145">
         <v>25.19</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="146">
         <v>37.78</v>
       </c>
-      <c r="I17" s="92">
+      <c r="I17" s="146">
         <v>88023.83</v>
       </c>
-      <c r="J17" s="92">
+      <c r="J17" s="133">
         <v>149436.59</v>
       </c>
-      <c r="K17" s="92">
-        <v>0</v>
-      </c>
-      <c r="L17" s="92">
+      <c r="L17" s="157">
         <v>1800</v>
       </c>
-      <c r="M17" s="92">
-        <v>0</v>
-      </c>
-      <c r="N17" s="92">
+      <c r="M17" s="159">
+        <v>0</v>
+      </c>
+      <c r="N17" s="145">
         <v>92616.29</v>
       </c>
-      <c r="O17" s="92">
+      <c r="O17" s="146">
         <v>149766.94</v>
       </c>
       <c r="P17" s="92">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="163">
+        <f t="shared" si="2"/>
+        <v>45342</v>
+      </c>
+      <c r="S17" s="165">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U17" s="165">
+        <f t="shared" si="4"/>
+        <v>3172.6669999999999</v>
+      </c>
+      <c r="V17" s="159"/>
+      <c r="W17" s="159"/>
+      <c r="X17" s="159"/>
+      <c r="Y17" s="159"/>
+      <c r="Z17" s="159"/>
+      <c r="AA17" s="159"/>
+      <c r="AB17" s="157"/>
+      <c r="AC17" s="159"/>
+      <c r="AD17" s="159"/>
+      <c r="AE17" s="159"/>
+      <c r="AH17" s="135">
+        <f t="shared" si="5"/>
+        <v>48514.667000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="99">
+      <c r="D18" s="144">
         <v>30115</v>
       </c>
-      <c r="E18" s="100">
+      <c r="E18" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>40.506849315068493</v>
       </c>
-      <c r="F18" s="97">
+      <c r="F18" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
-      <c r="G18" s="92">
+      <c r="G18" s="145">
         <v>39.46</v>
       </c>
-      <c r="H18" s="92">
+      <c r="H18" s="146">
         <v>59.19</v>
       </c>
-      <c r="I18" s="92">
+      <c r="I18" s="146">
         <v>92465.44</v>
       </c>
-      <c r="J18" s="92">
+      <c r="J18" s="133">
         <v>188016.91</v>
       </c>
-      <c r="K18" s="92">
-        <v>0</v>
-      </c>
-      <c r="L18" s="92">
+      <c r="L18" s="157">
         <v>1650</v>
       </c>
-      <c r="M18" s="92">
+      <c r="M18" s="159">
         <v>143.27000000000001</v>
       </c>
-      <c r="N18" s="92">
+      <c r="N18" s="145">
         <v>86538.68</v>
       </c>
-      <c r="O18" s="92">
+      <c r="O18" s="146">
         <v>168507.1</v>
       </c>
       <c r="P18" s="92">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="163">
+        <f t="shared" si="2"/>
+        <v>65109</v>
+      </c>
+      <c r="S18" s="165">
+        <f t="shared" si="3"/>
+        <v>8480.1512999999995</v>
+      </c>
+      <c r="T18" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U18" s="165">
+        <f t="shared" si="4"/>
+        <v>3392.9933000000001</v>
+      </c>
+      <c r="V18" s="159"/>
+      <c r="W18" s="159"/>
+      <c r="X18" s="159"/>
+      <c r="Y18" s="159"/>
+      <c r="Z18" s="159"/>
+      <c r="AA18" s="159"/>
+      <c r="AB18" s="157"/>
+      <c r="AC18" s="159"/>
+      <c r="AD18" s="159"/>
+      <c r="AE18" s="159"/>
+      <c r="AH18" s="135">
+        <f t="shared" si="5"/>
+        <v>76982.1446</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="99">
+      <c r="D19" s="144">
         <v>41231</v>
       </c>
-      <c r="E19" s="100">
+      <c r="E19" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>10.052054794520547</v>
       </c>
-      <c r="F19" s="97">
+      <c r="F19" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="G19" s="92">
+      <c r="G19" s="145">
         <v>15.1</v>
       </c>
-      <c r="H19" s="92">
+      <c r="H19" s="146">
         <v>22.64</v>
       </c>
-      <c r="I19" s="92">
+      <c r="I19" s="146">
         <v>82233.27</v>
       </c>
-      <c r="J19" s="92">
+      <c r="J19" s="133">
         <v>114677.5</v>
       </c>
-      <c r="K19" s="92">
-        <v>0</v>
-      </c>
-      <c r="L19" s="92">
+      <c r="L19" s="157">
         <v>1875</v>
       </c>
-      <c r="M19" s="92">
-        <v>0</v>
-      </c>
-      <c r="N19" s="92">
+      <c r="M19" s="159">
+        <v>0</v>
+      </c>
+      <c r="N19" s="145">
         <v>74240.86</v>
       </c>
-      <c r="O19" s="92">
+      <c r="O19" s="146">
         <v>112740.09</v>
       </c>
       <c r="P19" s="92">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R19" s="163">
+        <f t="shared" si="2"/>
+        <v>28312.5</v>
+      </c>
+      <c r="S19" s="165">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U19" s="165">
+        <f t="shared" si="4"/>
+        <v>2433.5099499999997</v>
+      </c>
+      <c r="V19" s="159"/>
+      <c r="W19" s="159"/>
+      <c r="X19" s="159"/>
+      <c r="Y19" s="159"/>
+      <c r="Z19" s="159"/>
+      <c r="AA19" s="159"/>
+      <c r="AB19" s="157"/>
+      <c r="AC19" s="159"/>
+      <c r="AD19" s="159"/>
+      <c r="AE19" s="159"/>
+      <c r="AH19" s="135">
+        <f t="shared" si="5"/>
+        <v>30746.00995</v>
+      </c>
+    </row>
+    <row r="20" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="99">
+      <c r="D20" s="144">
         <v>31824</v>
       </c>
-      <c r="E20" s="100">
+      <c r="E20" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>35.824657534246576</v>
       </c>
-      <c r="F20" s="97">
+      <c r="F20" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
-      <c r="G20" s="92">
+      <c r="G20" s="145">
         <v>35.71</v>
       </c>
-      <c r="H20" s="92">
+      <c r="H20" s="146">
         <v>53.57</v>
       </c>
-      <c r="I20" s="92">
+      <c r="I20" s="146">
         <v>91406.45</v>
       </c>
-      <c r="J20" s="92">
+      <c r="J20" s="133">
         <v>178594.61</v>
       </c>
-      <c r="K20" s="92">
-        <v>0</v>
-      </c>
-      <c r="L20" s="92">
+      <c r="L20" s="157">
         <v>1687.5</v>
       </c>
-      <c r="M20" s="92">
+      <c r="M20" s="159">
         <v>145.13</v>
       </c>
-      <c r="N20" s="92">
+      <c r="N20" s="145">
         <v>90744.11</v>
       </c>
-      <c r="O20" s="92">
+      <c r="O20" s="146">
         <v>180217.79</v>
       </c>
       <c r="P20" s="92">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R20" s="163">
+        <f t="shared" si="2"/>
+        <v>60260.625</v>
+      </c>
+      <c r="S20" s="165">
+        <f t="shared" si="3"/>
+        <v>7774.6140999999998</v>
+      </c>
+      <c r="T20" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U20" s="165">
+        <f t="shared" si="4"/>
+        <v>3610.70795</v>
+      </c>
+      <c r="V20" s="159"/>
+      <c r="W20" s="159"/>
+      <c r="X20" s="159"/>
+      <c r="Y20" s="159"/>
+      <c r="Z20" s="159"/>
+      <c r="AA20" s="159"/>
+      <c r="AB20" s="157"/>
+      <c r="AC20" s="159"/>
+      <c r="AD20" s="159"/>
+      <c r="AE20" s="159"/>
+      <c r="AH20" s="135">
+        <f t="shared" si="5"/>
+        <v>71645.947050000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="99">
+      <c r="D21" s="144">
         <v>38150</v>
       </c>
-      <c r="E21" s="100">
+      <c r="E21" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>18.493150684931507</v>
       </c>
-      <c r="F21" s="97">
+      <c r="F21" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="G21" s="92">
+      <c r="G21" s="145">
         <v>21.85</v>
       </c>
-      <c r="H21" s="92">
+      <c r="H21" s="146">
         <v>32.770000000000003</v>
       </c>
-      <c r="I21" s="92">
+      <c r="I21" s="146">
         <v>86792.81</v>
       </c>
-      <c r="J21" s="92">
+      <c r="J21" s="133">
         <v>139268.84</v>
       </c>
-      <c r="K21" s="92">
-        <v>0</v>
-      </c>
-      <c r="L21" s="92">
+      <c r="L21" s="157">
         <v>1837.5</v>
       </c>
-      <c r="M21" s="92">
+      <c r="M21" s="159">
         <v>191.85</v>
       </c>
-      <c r="N21" s="92">
+      <c r="N21" s="145">
         <v>92277.83</v>
       </c>
-      <c r="O21" s="92">
+      <c r="O21" s="146">
         <v>139124.15</v>
       </c>
       <c r="P21" s="92">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="163">
+        <f t="shared" si="2"/>
+        <v>40149.375</v>
+      </c>
+      <c r="S21" s="165">
+        <f t="shared" si="3"/>
+        <v>6286.9245000000001</v>
+      </c>
+      <c r="T21" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U21" s="165">
+        <f t="shared" si="4"/>
+        <v>3009.6405499999996</v>
+      </c>
+      <c r="V21" s="159"/>
+      <c r="W21" s="159"/>
+      <c r="X21" s="159"/>
+      <c r="Y21" s="159"/>
+      <c r="Z21" s="159"/>
+      <c r="AA21" s="159"/>
+      <c r="AB21" s="157"/>
+      <c r="AC21" s="159"/>
+      <c r="AD21" s="159"/>
+      <c r="AE21" s="159"/>
+      <c r="AH21" s="135">
+        <f t="shared" si="5"/>
+        <v>49445.940049999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="99">
+      <c r="D22" s="144">
         <v>32891</v>
       </c>
-      <c r="E22" s="100">
+      <c r="E22" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>32.901369863013699</v>
       </c>
-      <c r="F22" s="97">
+      <c r="F22" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
-      <c r="G22" s="92">
+      <c r="G22" s="145">
         <v>33.380000000000003</v>
       </c>
-      <c r="H22" s="92">
+      <c r="H22" s="146">
         <v>50.06</v>
       </c>
-      <c r="I22" s="92">
+      <c r="I22" s="146">
         <v>91420.63</v>
       </c>
-      <c r="J22" s="92">
+      <c r="J22" s="133">
         <v>173822.75</v>
       </c>
-      <c r="K22" s="92">
-        <v>0</v>
-      </c>
-      <c r="L22" s="92">
+      <c r="L22" s="157">
         <v>1725</v>
       </c>
-      <c r="M22" s="92">
+      <c r="M22" s="159">
         <v>150.72</v>
       </c>
-      <c r="N22" s="92">
+      <c r="N22" s="145">
         <v>80527.14</v>
       </c>
-      <c r="O22" s="92">
+      <c r="O22" s="146">
         <v>181545.58</v>
       </c>
       <c r="P22" s="92">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="163">
+        <f t="shared" si="2"/>
+        <v>57580.500000000007</v>
+      </c>
+      <c r="S22" s="165">
+        <f t="shared" si="3"/>
+        <v>7545.0432000000001</v>
+      </c>
+      <c r="T22" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U22" s="165">
+        <f t="shared" si="4"/>
+        <v>3528.4550999999997</v>
+      </c>
+      <c r="V22" s="159"/>
+      <c r="W22" s="159"/>
+      <c r="X22" s="159"/>
+      <c r="Y22" s="159"/>
+      <c r="Z22" s="159"/>
+      <c r="AA22" s="159"/>
+      <c r="AB22" s="157"/>
+      <c r="AC22" s="159"/>
+      <c r="AD22" s="159"/>
+      <c r="AE22" s="159"/>
+      <c r="AH22" s="135">
+        <f t="shared" si="5"/>
+        <v>68653.998300000007</v>
+      </c>
+    </row>
+    <row r="23" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="99">
+      <c r="D23" s="144">
         <v>41102</v>
       </c>
-      <c r="E23" s="100">
+      <c r="E23" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>10.405479452054795</v>
       </c>
-      <c r="F23" s="97">
+      <c r="F23" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="G23" s="92">
+      <c r="G23" s="145">
         <v>15.38</v>
       </c>
-      <c r="H23" s="92">
+      <c r="H23" s="146">
         <v>23.07</v>
       </c>
-      <c r="I23" s="92">
+      <c r="I23" s="146">
         <v>82498.34</v>
       </c>
-      <c r="J23" s="92">
+      <c r="J23" s="133">
         <v>115826.13</v>
       </c>
-      <c r="K23" s="92">
-        <v>0</v>
-      </c>
-      <c r="L23" s="92">
+      <c r="L23" s="157">
         <v>1875</v>
       </c>
-      <c r="M23" s="92">
+      <c r="M23" s="159">
         <v>159.16999999999999</v>
       </c>
-      <c r="N23" s="92">
+      <c r="N23" s="145">
         <v>73878.58</v>
       </c>
-      <c r="O23" s="92">
+      <c r="O23" s="146">
         <v>125469.62</v>
       </c>
       <c r="P23" s="92">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="2:18" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="163">
+        <f t="shared" si="2"/>
+        <v>28837.5</v>
+      </c>
+      <c r="S23" s="165">
+        <f t="shared" si="3"/>
+        <v>3672.0518999999999</v>
+      </c>
+      <c r="T23" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U23" s="165">
+        <f t="shared" si="4"/>
+        <v>2620.8300999999997</v>
+      </c>
+      <c r="V23" s="159"/>
+      <c r="W23" s="159"/>
+      <c r="X23" s="159"/>
+      <c r="Y23" s="159"/>
+      <c r="Z23" s="159"/>
+      <c r="AA23" s="159"/>
+      <c r="AB23" s="157"/>
+      <c r="AC23" s="159"/>
+      <c r="AD23" s="159"/>
+      <c r="AE23" s="159"/>
+      <c r="AH23" s="135">
+        <f t="shared" si="5"/>
+        <v>35130.381999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="96" t="s">
+      <c r="C24" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="99">
+      <c r="D24" s="144">
         <v>29465</v>
       </c>
-      <c r="E24" s="100">
+      <c r="E24" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>42.287671232876711</v>
       </c>
-      <c r="F24" s="97">
+      <c r="F24" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
-      <c r="G24" s="92">
+      <c r="G24" s="145">
         <v>40.880000000000003</v>
       </c>
-      <c r="H24" s="92">
+      <c r="H24" s="146">
         <v>61.33</v>
       </c>
-      <c r="I24" s="92">
+      <c r="I24" s="146">
         <v>93640.78</v>
       </c>
-      <c r="J24" s="92">
+      <c r="J24" s="133">
         <v>193110.06</v>
       </c>
-      <c r="K24" s="92">
-        <v>0</v>
-      </c>
-      <c r="L24" s="92">
+      <c r="L24" s="157">
         <v>1650</v>
       </c>
-      <c r="M24" s="92">
-        <v>0</v>
-      </c>
-      <c r="N24" s="92">
+      <c r="M24" s="159">
+        <v>0</v>
+      </c>
+      <c r="N24" s="145">
         <v>83732.44</v>
       </c>
-      <c r="O24" s="92">
+      <c r="O24" s="146">
         <v>208951.82</v>
       </c>
       <c r="P24" s="92">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R24" s="163">
+        <f t="shared" si="2"/>
+        <v>67452</v>
+      </c>
+      <c r="S24" s="165">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U24" s="165">
+        <f t="shared" si="4"/>
+        <v>3971.6017000000002</v>
+      </c>
+      <c r="V24" s="159"/>
+      <c r="W24" s="159"/>
+      <c r="X24" s="159"/>
+      <c r="Y24" s="159"/>
+      <c r="Z24" s="159"/>
+      <c r="AA24" s="159"/>
+      <c r="AB24" s="157"/>
+      <c r="AC24" s="159"/>
+      <c r="AD24" s="159"/>
+      <c r="AE24" s="159"/>
+      <c r="AH24" s="135">
+        <f t="shared" si="5"/>
+        <v>71423.601699999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="96" t="s">
+      <c r="C25" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="99">
+      <c r="D25" s="144">
         <v>30711</v>
       </c>
-      <c r="E25" s="100">
+      <c r="E25" s="152">
         <f t="shared" ca="1" si="0"/>
         <v>38.873972602739727</v>
       </c>
-      <c r="F25" s="97">
+      <c r="F25" s="153">
         <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
-      <c r="G25" s="92">
+      <c r="G25" s="145">
         <v>38.15</v>
       </c>
-      <c r="H25" s="92">
+      <c r="H25" s="146">
         <v>57.23</v>
       </c>
-      <c r="I25" s="92">
+      <c r="I25" s="146">
         <v>93464.74</v>
       </c>
-      <c r="J25" s="92">
+      <c r="J25" s="133">
         <v>187513.86</v>
       </c>
-      <c r="K25" s="92">
-        <v>0</v>
-      </c>
-      <c r="L25" s="92">
+      <c r="L25" s="157">
         <v>1687.5</v>
       </c>
-      <c r="M25" s="92">
+      <c r="M25" s="159">
         <v>226.41</v>
       </c>
-      <c r="N25" s="92">
+      <c r="N25" s="145">
         <v>98278.63</v>
       </c>
-      <c r="O25" s="92">
+      <c r="O25" s="146">
         <v>171337.91</v>
       </c>
       <c r="P25" s="92">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R25" s="163">
+        <f t="shared" si="2"/>
+        <v>64378.125</v>
+      </c>
+      <c r="S25" s="165">
+        <f t="shared" si="3"/>
+        <v>12957.444299999999</v>
+      </c>
+      <c r="T25" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="U25" s="165">
+        <f t="shared" si="4"/>
+        <v>3552.8549500000004</v>
+      </c>
+      <c r="V25" s="159"/>
+      <c r="W25" s="159"/>
+      <c r="X25" s="159"/>
+      <c r="Y25" s="159"/>
+      <c r="Z25" s="159"/>
+      <c r="AA25" s="159"/>
+      <c r="AB25" s="157"/>
+      <c r="AC25" s="159"/>
+      <c r="AD25" s="159"/>
+      <c r="AE25" s="159"/>
+      <c r="AH25" s="135">
+        <f t="shared" si="5"/>
+        <v>80888.424249999996</v>
+      </c>
+    </row>
+    <row r="26" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="135">
+        <f>SUM(I9:I25)</f>
+        <v>1508346.0400000003</v>
+      </c>
+      <c r="J26" s="135">
+        <f>SUM(J9:J25)</f>
+        <v>2659832.84</v>
+      </c>
+      <c r="N26" s="135">
+        <f>SUM(N9:N25)</f>
+        <v>1486480.73</v>
+      </c>
+      <c r="O26" s="135">
+        <f>SUM(O9:O25)</f>
+        <v>2596154.92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B29" s="92" t="s">
         <v>12</v>
       </c>
@@ -6013,16 +6755,21 @@
       <c r="G29" s="92" t="s">
         <v>12</v>
       </c>
+      <c r="I29" s="134"/>
       <c r="R29" s="92" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:18" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:34" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="19">
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AD7:AE7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="B5:J6"/>
     <mergeCell ref="L5:P6"/>
@@ -6033,10 +6780,40 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
   </mergeCells>
+  <conditionalFormatting sqref="B9:J25">
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:P25">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R9:AH25">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E9:E25 F9:F25" unlockedFormula="1"/>
+    <ignoredError sqref="E9:E25 F9:F25 I26:J26 N26:O26 R9:R25 S9:S25 U9 AH9:AH25 U10:U25" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6061,15 +6838,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="129" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="130" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="88" t="s">
@@ -6077,25 +6854,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="142"/>
+      <c r="C5" s="131"/>
       <c r="D5" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="142"/>
+      <c r="C6" s="131"/>
       <c r="D6" s="71" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="142"/>
+      <c r="C7" s="131"/>
       <c r="D7" s="70" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="143"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="89" t="s">
         <v>56</v>
       </c>
@@ -6115,7 +6892,7 @@
       <c r="C11" s="72"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="141" t="s">
+      <c r="C12" s="130" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="88" t="s">
@@ -6123,43 +6900,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="142"/>
+      <c r="C13" s="131"/>
       <c r="D13" s="70" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="142"/>
+      <c r="C14" s="131"/>
       <c r="D14" s="68" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="142"/>
+      <c r="C15" s="131"/>
       <c r="D15" s="87" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="142"/>
+      <c r="C16" s="131"/>
       <c r="D16" s="68" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="142"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="87" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="142"/>
+      <c r="C18" s="131"/>
       <c r="D18" s="68" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="143"/>
+      <c r="C19" s="132"/>
       <c r="D19" s="89" t="s">
         <v>61</v>
       </c>

</xml_diff>